<commit_message>
Inicio Relatorio Vig. Epid
</commit_message>
<xml_diff>
--- a/Dispensação x Agravo/Incorreto Dispensacoes x Agravos.xlsx
+++ b/Dispensação x Agravo/Incorreto Dispensacoes x Agravos.xlsx
@@ -1,32 +1,19 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,13 +32,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -336,16 +390,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>